<commit_message>
updated sillbanta assignment clinic.xlsx after the instruction
</commit_message>
<xml_diff>
--- a/Skillbanta Assignment Clinic.xlsx
+++ b/Skillbanta Assignment Clinic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Desktop\Skilbanta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B268A4-DDB9-4A1F-83C1-33E304575919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607CA94C-559A-4F1F-B7E8-BB5ED76429B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="15" xr2:uid="{22EB0AF4-8C10-4F5E-840B-5B23863D520D}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="745">
   <si>
     <t>Use Cases</t>
   </si>
@@ -401,9 +401,6 @@
       </rPr>
       <t>https://clinicbookingportal.com/signup</t>
     </r>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Scenario 2: OTP Generation on Signup</t>
@@ -2789,10 +2786,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114D185D-C85B-4D09-8EEC-898349E482AC}">
-  <dimension ref="C1:I13"/>
+  <dimension ref="C1:H13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2805,12 +2802,12 @@
     <col min="8" max="8" width="29.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="1" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C1" s="7" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.45">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
@@ -2829,208 +2826,205 @@
       <c r="H3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" ht="81" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="3:8" ht="81" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="10" t="s">
+        <v>477</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="G4" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="93" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="108" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="120.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="131.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
+        <v>495</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F8" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>456</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="120.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>459</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>460</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>482</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>495</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" ht="131.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="107.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" ht="107.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>497</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="F9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="F10" s="10" t="s">
+    </row>
+    <row r="11" spans="3:8" ht="112.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" ht="112.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="F11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="103.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>502</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" ht="103.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="F12" s="10" t="s">
+    </row>
+    <row r="13" spans="3:8" ht="129.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>504</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" ht="129.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>475</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="G13" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>476</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>488</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -3040,7 +3034,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21237D34-F740-4F44-851B-CBEEA7F0A3EC}">
-  <dimension ref="C1:I13"/>
+  <dimension ref="C1:H13"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
@@ -3056,12 +3050,12 @@
     <col min="8" max="8" width="35.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="1" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C1" s="7" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.45">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
@@ -3080,208 +3074,205 @@
       <c r="H3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" ht="83.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="3:8" ht="83.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="H4" s="10" t="s">
+    </row>
+    <row r="5" spans="3:8" ht="127.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" ht="127.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="10" t="s">
-        <v>558</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="H5" s="10" t="s">
+    </row>
+    <row r="6" spans="3:8" ht="114.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>518</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="H6" s="10" t="s">
+    </row>
+    <row r="7" spans="3:8" ht="100.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" ht="100.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="10" t="s">
-        <v>568</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="100.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" ht="100.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
-        <v>573</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>525</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>526</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>528</v>
       </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="94.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" ht="94.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>530</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>530</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>508</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>531</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>532</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="E10" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>578</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>534</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>535</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>536</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="H10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="E11" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>539</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="95.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>579</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>538</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>539</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="H11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" ht="95.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="H12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
-        <v>581</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>549</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -3292,7 +3283,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EB3139-63DE-4B87-B115-64F6CFE424C4}">
-  <dimension ref="C1:I9"/>
+  <dimension ref="C1:H9"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
@@ -3308,12 +3299,12 @@
     <col min="8" max="8" width="27.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="1" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="D1" s="7" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.45">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C4" s="8" t="s">
         <v>55</v>
       </c>
@@ -3332,108 +3323,105 @@
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="3:8" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>554</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="120.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>553</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="115.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="103.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="120.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="10" t="s">
-        <v>583</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>559</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>560</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>561</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="146.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" ht="115.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
-        <v>585</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>569</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>570</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>571</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" ht="103.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
-        <v>586</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>574</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>575</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -3444,7 +3432,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430ABDB2-7A9B-4BA6-8E07-FC14CF3D20E0}">
-  <dimension ref="C1:S32"/>
+  <dimension ref="C1:R32"/>
   <sheetViews>
     <sheetView topLeftCell="E4" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
@@ -3460,12 +3448,12 @@
     <col min="9" max="9" width="44.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:19" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="1" spans="3:18" ht="22.9" x14ac:dyDescent="0.6">
       <c r="D1" s="7" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.45">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -3482,9 +3470,8 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.45">
       <c r="D5" s="8" t="s">
         <v>55</v>
       </c>
@@ -3503,29 +3490,26 @@
       <c r="I5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="3:19" ht="94.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="3:18" ht="94.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="2"/>
       <c r="D6" s="10" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>588</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>589</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>590</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>591</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>592</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -3536,27 +3520,26 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-    </row>
-    <row r="7" spans="3:19" ht="84.4" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:18" ht="84.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="2"/>
       <c r="D7" s="10" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>594</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>595</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>596</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>597</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>598</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -3567,27 +3550,26 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="3:19" ht="91.9" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="3:18" ht="91.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" s="2"/>
       <c r="D8" s="10" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>600</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>589</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>601</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>602</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>603</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -3598,27 +3580,26 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="3:19" ht="88.9" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="3:18" ht="88.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C9" s="2"/>
       <c r="D9" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>589</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>606</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>607</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>608</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -3629,27 +3610,26 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="3:19" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="3:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C10" s="2"/>
       <c r="D10" s="10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>611</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>591</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>612</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -3660,27 +3640,26 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="3:19" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="3:18" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C11" s="2"/>
       <c r="D11" s="10" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>613</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>614</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>615</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>616</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>617</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -3691,9 +3670,8 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -3710,9 +3688,8 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -3729,9 +3706,8 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -3748,9 +3724,8 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -3767,9 +3742,8 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -3786,9 +3760,8 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3805,9 +3778,8 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -3824,9 +3796,8 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -3843,9 +3814,8 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -3862,9 +3832,8 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -3881,9 +3850,8 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -3900,9 +3868,8 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -3919,9 +3886,8 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-    </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -3938,9 +3904,8 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -3957,9 +3922,8 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-    </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -3976,9 +3940,8 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-    </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -3995,9 +3958,8 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-    </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -4014,9 +3976,8 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-    </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -4033,9 +3994,8 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-    </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -4052,9 +4012,8 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-    </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -4071,9 +4030,8 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-    </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -4090,7 +4048,6 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4100,7 +4057,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9596DCB-B146-4530-9E1C-4B452EED1D02}">
-  <dimension ref="D1:J13"/>
+  <dimension ref="D1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -4116,12 +4073,12 @@
     <col min="9" max="9" width="24.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="1" spans="4:9" ht="22.9" x14ac:dyDescent="0.6">
       <c r="E1" s="7" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.45">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D3" s="8" t="s">
         <v>55</v>
       </c>
@@ -4140,208 +4097,205 @@
       <c r="I3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="4:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="4:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D4" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>623</v>
       </c>
-      <c r="I4" s="10" t="s">
+    </row>
+    <row r="5" spans="4:9" ht="117.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D5" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="5" spans="4:10" ht="117.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="10" t="s">
-        <v>593</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>626</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>627</v>
       </c>
-      <c r="I5" s="10" t="s">
+    </row>
+    <row r="6" spans="4:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D6" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="6" spans="4:10" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="10" t="s">
-        <v>599</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>631</v>
       </c>
-      <c r="I6" s="10" t="s">
+    </row>
+    <row r="7" spans="4:9" ht="109.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D7" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="7" spans="4:10" ht="109.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D7" s="10" t="s">
-        <v>604</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>633</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>635</v>
       </c>
-      <c r="I7" s="10" t="s">
+    </row>
+    <row r="8" spans="4:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D8" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="8" spans="4:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D8" s="10" t="s">
-        <v>609</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>638</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="I8" s="10" t="s">
+    </row>
+    <row r="9" spans="4:9" ht="88.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="9" spans="4:10" ht="88.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D9" s="10" t="s">
-        <v>613</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>641</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>642</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D10" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>643</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D10" s="10" t="s">
+      <c r="F10" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>645</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" ht="120.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D11" s="10" t="s">
         <v>665</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>645</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>646</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="11" spans="4:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D11" s="10" t="s">
+      <c r="F11" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="97.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D12" s="10" t="s">
         <v>666</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>648</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>649</v>
-      </c>
-      <c r="H11" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>650</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D13" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>656</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>623</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" ht="97.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D12" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>651</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>623</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="13" spans="4:10" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D13" s="10" t="s">
-        <v>668</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>623</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -4352,7 +4306,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7D63C1-11FD-4797-935E-219976AE5EC9}">
-  <dimension ref="C2:I16"/>
+  <dimension ref="C2:H16"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
@@ -4366,15 +4320,14 @@
     <col min="6" max="6" width="42.9296875" customWidth="1"/>
     <col min="7" max="7" width="37.796875" customWidth="1"/>
     <col min="8" max="8" width="46.19921875" customWidth="1"/>
-    <col min="9" max="9" width="14.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="2" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -4393,208 +4346,205 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="66" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="66" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>670</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>671</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>672</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>673</v>
       </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>675</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>676</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="H8" s="10" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>672</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>678</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
-        <v>680</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>681</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>682</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>683</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>673</v>
-      </c>
-      <c r="H9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="72.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" ht="72.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>685</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>686</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>687</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>688</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>673</v>
-      </c>
-      <c r="H10" s="10" t="s">
+    </row>
+    <row r="11" spans="3:8" ht="85.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" ht="85.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>690</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>693</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>694</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="91.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" ht="91.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>696</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>698</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>673</v>
-      </c>
-      <c r="H12" s="10" t="s">
+    </row>
+    <row r="13" spans="3:8" ht="83.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" ht="83.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>702</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>703</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>705</v>
       </c>
-      <c r="H13" s="10" t="s">
+    </row>
+    <row r="14" spans="3:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="10" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>707</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>708</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>709</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>710</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>673</v>
-      </c>
-      <c r="H14" s="10" t="s">
+    </row>
+    <row r="15" spans="3:8" ht="96" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" ht="96" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>712</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>713</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>714</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>715</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>716</v>
       </c>
-      <c r="H15" s="10" t="s">
+    </row>
+    <row r="16" spans="3:8" ht="96.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" ht="96.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>718</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>719</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>720</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>721</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>722</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -4604,9 +4554,9 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81533E9-07BA-4B74-885D-EB3DD2E40B40}">
-  <dimension ref="C1:I9"/>
+  <dimension ref="C1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -4620,12 +4570,12 @@
     <col min="8" max="8" width="28.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="1" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C4" s="8" t="s">
         <v>55</v>
       </c>
@@ -4644,108 +4594,105 @@
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="3:8" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>724</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>725</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>726</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>727</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="H5" s="10" t="s">
+    </row>
+    <row r="6" spans="3:8" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="10" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>729</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>730</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>727</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>732</v>
       </c>
-      <c r="H6" s="10" t="s">
+    </row>
+    <row r="7" spans="3:8" ht="95.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="10" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>734</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>574</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>736</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="117.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>738</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>739</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>740</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>741</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="114.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>743</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>744</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>698</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>745</v>
-      </c>
       <c r="G9" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -4757,7 +4704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD9A732-3F0A-48AC-88DC-52CE63977BA6}">
   <dimension ref="C5:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -4963,10 +4910,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4354996-AC1E-4754-B560-C1319C74BF5E}">
-  <dimension ref="C4:I16"/>
+  <dimension ref="C4:H16"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4979,7 +4926,7 @@
     <col min="8" max="8" width="24.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C4" s="7" t="s">
         <v>54</v>
       </c>
@@ -4989,7 +4936,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -4997,7 +4944,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="3:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -5016,11 +4963,8 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="81.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
         <v>61</v>
       </c>
@@ -5040,7 +4984,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="3:9" ht="94.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:8" ht="94.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" s="10" t="s">
         <v>66</v>
       </c>
@@ -5060,7 +5004,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="3:9" ht="78" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:8" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C9" s="10" t="s">
         <v>71</v>
       </c>
@@ -5080,7 +5024,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="3:9" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:8" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C10" s="10" t="s">
         <v>76</v>
       </c>
@@ -5100,7 +5044,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="3:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C11" s="10" t="s">
         <v>81</v>
       </c>
@@ -5120,7 +5064,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="3:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C12" s="10" t="s">
         <v>85</v>
       </c>
@@ -5140,7 +5084,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="3:9" ht="83.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:8" ht="83.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" s="10" t="s">
         <v>90</v>
       </c>
@@ -5160,7 +5104,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="3:9" ht="105.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:8" ht="105.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" s="10" t="s">
         <v>94</v>
       </c>
@@ -5180,7 +5124,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="3:9" ht="112.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:8" ht="112.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="10" t="s">
         <v>99</v>
       </c>
@@ -5200,7 +5144,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="3:9" ht="63.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:8" ht="63.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C16" s="10" t="s">
         <v>103</v>
       </c>
@@ -5227,10 +5171,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BC240D-537E-4BA2-B882-468A6195CACF}">
-  <dimension ref="C4:I16"/>
+  <dimension ref="C4:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5241,30 +5185,27 @@
     <col min="6" max="6" width="30.1328125" customWidth="1"/>
     <col min="7" max="7" width="27.1328125" customWidth="1"/>
     <col min="8" max="8" width="28.9296875" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -5283,219 +5224,206 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="3:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="71.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="3:9" ht="71.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="63.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="3:9" ht="63.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="3:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="78" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="3:9" ht="78" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="H12" s="10" t="s">
+    </row>
+    <row r="13" spans="3:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="3:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="H13" s="10" t="s">
+    </row>
+    <row r="14" spans="3:8" ht="53.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="3:9" ht="53.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F14" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="H14" s="10" t="s">
+    </row>
+    <row r="15" spans="3:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="3:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="H15" s="10" t="s">
+    </row>
+    <row r="16" spans="3:8" ht="51.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="3:9" ht="51.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="I16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5504,10 +5432,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FAC04F-CB27-4239-A20E-B9084EB0C747}">
-  <dimension ref="C4:I16"/>
+  <dimension ref="C4:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5518,15 +5446,14 @@
     <col min="6" max="6" width="25.06640625" customWidth="1"/>
     <col min="7" max="7" width="21.06640625" customWidth="1"/>
     <col min="8" max="8" width="39.86328125" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C4" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="27" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="27" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -5545,219 +5472,206 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="3:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="85.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="3:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="H9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="99" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="3:9" ht="99" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="H10" s="10" t="s">
+    </row>
+    <row r="11" spans="3:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="3:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F11" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="101.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="3:9" ht="101.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="H12" s="10" t="s">
+    </row>
+    <row r="13" spans="3:8" ht="96.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="3:9" ht="96.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="H13" s="10" t="s">
+    </row>
+    <row r="14" spans="3:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="3:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="H14" s="10" t="s">
+    </row>
+    <row r="15" spans="3:8" ht="107.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="3:9" ht="107.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" s="10" t="s">
+    </row>
+    <row r="16" spans="3:8" ht="84" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="3:9" ht="84" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="I16" s="2"/>
+        <v>224</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5766,9 +5680,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4543C387-B3A5-486B-BBD3-75A263582E7A}">
-  <dimension ref="B4:H16"/>
+  <dimension ref="B4:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -5780,30 +5694,27 @@
     <col min="5" max="5" width="38.46484375" customWidth="1"/>
     <col min="6" max="6" width="30.06640625" customWidth="1"/>
     <col min="7" max="7" width="40.19921875" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:7" ht="22.9" x14ac:dyDescent="0.6">
       <c r="B4" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:8" ht="88.9" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="2:7" ht="88.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="s">
         <v>55</v>
       </c>
@@ -5822,219 +5733,206 @@
       <c r="G6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="2:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>230</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="G8" s="10" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="G9" s="10" t="s">
+    </row>
+    <row r="10" spans="2:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="G10" s="10" t="s">
+    </row>
+    <row r="11" spans="2:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="G11" s="10" t="s">
+    </row>
+    <row r="12" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G12" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="56.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G13" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="61.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:8" ht="61.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>266</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>271</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G15" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>273</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>274</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="H16" s="2"/>
+        <v>275</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6043,10 +5941,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF7299C-DD19-4C16-BCCC-85C5A9B814B2}">
-  <dimension ref="C4:I16"/>
+  <dimension ref="C4:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6059,9 +5957,9 @@
     <col min="8" max="8" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C4" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -6069,7 +5967,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -6077,7 +5975,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -6096,208 +5994,205 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="57.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" ht="57.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="H9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="H10" s="10" t="s">
+    </row>
+    <row r="11" spans="3:8" ht="67.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" ht="67.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="85.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="H12" s="10" t="s">
+    </row>
+    <row r="13" spans="3:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="H13" s="10" t="s">
+    </row>
+    <row r="14" spans="3:8" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="10" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="H14" s="10" t="s">
+    </row>
+    <row r="15" spans="3:8" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="H15" s="10" t="s">
+    </row>
+    <row r="16" spans="3:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>334</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>335</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -6308,10 +6203,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B211C65-2354-43FE-B86B-4145FA79F7C6}">
-  <dimension ref="C4:I18"/>
+  <dimension ref="C4:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6324,9 +6219,9 @@
     <col min="8" max="8" width="54.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C4" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -6334,7 +6229,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -6342,7 +6237,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -6361,208 +6256,205 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:8" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" ht="75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="H9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="H10" s="10" t="s">
+    </row>
+    <row r="11" spans="3:8" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="H12" s="10" t="s">
+    </row>
+    <row r="13" spans="3:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="H13" s="10" t="s">
+    </row>
+    <row r="14" spans="3:8" ht="61.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="10" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" ht="61.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="H14" s="10" t="s">
+    </row>
+    <row r="15" spans="3:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="H15" s="10" t="s">
+    </row>
+    <row r="16" spans="3:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>393</v>
-      </c>
       <c r="H16" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.45">
@@ -6589,10 +6481,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8BE6F9-7DC0-4080-88BF-F6BA69945301}">
-  <dimension ref="C4:I16"/>
+  <dimension ref="C4:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6605,12 +6497,12 @@
     <col min="8" max="8" width="39.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="22.9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:8" ht="22.9" x14ac:dyDescent="0.6">
       <c r="C4" s="7" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
@@ -6629,208 +6521,205 @@
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="3:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>397</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>398</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>69</v>
       </c>
       <c r="H7" s="10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="H8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="H9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:8" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="10" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="H10" s="10" t="s">
+    </row>
+    <row r="11" spans="3:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="10" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="3:8" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>424</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>425</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>69</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="85.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="10" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" ht="85.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="H13" s="10" t="s">
+    </row>
+    <row r="14" spans="3:8" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="10" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="H14" s="10" t="s">
+    </row>
+    <row r="15" spans="3:8" ht="57.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" ht="57.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="H15" s="10" t="s">
+    </row>
+    <row r="16" spans="3:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>447</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>448</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>